<commit_message>
results template file for FERT, and updates to some other template files
</commit_message>
<xml_diff>
--- a/src/class_ALLERGY/results_template.xlsx
+++ b/src/class_ALLERGY/results_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\project\loinc-equivalence-classes\class_ALLERGY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\project\loinc-equivalence-classes\src\class_ALLERGY\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28530" windowHeight="16395"/>
   </bookViews>
   <sheets>
     <sheet name="group size &gt; 1" sheetId="1" r:id="rId1"/>
@@ -398,8 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,8 +449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>